<commit_message>
new changes - scn2 and scn3
</commit_message>
<xml_diff>
--- a/model_accuracy_log.xlsx
+++ b/model_accuracy_log.xlsx
@@ -390,7 +390,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E90"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -415,7 +415,7 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="2">
-        <v>45917.90277320537</v>
+        <v>45917.90277320602</v>
       </c>
       <c r="B2">
         <v>0.9943499860443238</v>
@@ -428,6 +428,1502 @@
       </c>
       <c r="E2">
         <v>61.13846686110924</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="2">
+        <v>45918.54004277778</v>
+      </c>
+      <c r="B3">
+        <v>0.9485591830944288</v>
+      </c>
+      <c r="C3">
+        <v>0.9498868332752911</v>
+      </c>
+      <c r="D3">
+        <v>8.289388564035244</v>
+      </c>
+      <c r="E3">
+        <v>7.385850170218077</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="2">
+        <v>45918.54059877315</v>
+      </c>
+      <c r="B4">
+        <v>0.998978224924668</v>
+      </c>
+      <c r="C4">
+        <v>0.9882305156116444</v>
+      </c>
+      <c r="D4">
+        <v>0.503087201070504</v>
+      </c>
+      <c r="E4">
+        <v>5.262627670368206</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" s="2">
+        <v>45918.54097726852</v>
+      </c>
+      <c r="B5">
+        <v>0.998978224924668</v>
+      </c>
+      <c r="C5">
+        <v>0.9882305156116444</v>
+      </c>
+      <c r="D5">
+        <v>0.503087201070504</v>
+      </c>
+      <c r="E5">
+        <v>5.262627670368206</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" s="2">
+        <v>45918.54115077546</v>
+      </c>
+      <c r="B6">
+        <v>0.998978224924668</v>
+      </c>
+      <c r="C6">
+        <v>0.9882305156116444</v>
+      </c>
+      <c r="D6">
+        <v>0.503087201070504</v>
+      </c>
+      <c r="E6">
+        <v>5.262627670368206</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" s="2">
+        <v>45918.54145944444</v>
+      </c>
+      <c r="B7">
+        <v>0.998978224924668</v>
+      </c>
+      <c r="C7">
+        <v>0.9882305156116444</v>
+      </c>
+      <c r="D7">
+        <v>0.503087201070504</v>
+      </c>
+      <c r="E7">
+        <v>5.262627670368206</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" s="2">
+        <v>45918.5439655787</v>
+      </c>
+      <c r="B8">
+        <v>0.998978224924668</v>
+      </c>
+      <c r="C8">
+        <v>0.9882305156116444</v>
+      </c>
+      <c r="D8">
+        <v>0.503087201070504</v>
+      </c>
+      <c r="E8">
+        <v>5.262627670368206</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" s="2">
+        <v>45918.54403443287</v>
+      </c>
+      <c r="B9">
+        <v>0.998978224924668</v>
+      </c>
+      <c r="C9">
+        <v>0.9882305156116444</v>
+      </c>
+      <c r="D9">
+        <v>0.503087201070504</v>
+      </c>
+      <c r="E9">
+        <v>5.262627670368206</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" s="2">
+        <v>45918.54474201389</v>
+      </c>
+      <c r="B10">
+        <v>0.998978224924668</v>
+      </c>
+      <c r="C10">
+        <v>0.9882305156116444</v>
+      </c>
+      <c r="D10">
+        <v>0.503087201070504</v>
+      </c>
+      <c r="E10">
+        <v>5.262627670368206</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" s="2">
+        <v>45918.54480730324</v>
+      </c>
+      <c r="B11">
+        <v>0.998978224924668</v>
+      </c>
+      <c r="C11">
+        <v>0.9882305156116444</v>
+      </c>
+      <c r="D11">
+        <v>0.503087201070504</v>
+      </c>
+      <c r="E11">
+        <v>5.262627670368206</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" s="2">
+        <v>45918.60519193287</v>
+      </c>
+      <c r="B12">
+        <v>0.998978224924668</v>
+      </c>
+      <c r="C12">
+        <v>0.9882305156116444</v>
+      </c>
+      <c r="D12">
+        <v>0.503087201070504</v>
+      </c>
+      <c r="E12">
+        <v>5.262627670368206</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" s="2">
+        <v>45918.60531452546</v>
+      </c>
+      <c r="B13">
+        <v>0.998978224924668</v>
+      </c>
+      <c r="C13">
+        <v>0.9882305156116444</v>
+      </c>
+      <c r="D13">
+        <v>0.503087201070504</v>
+      </c>
+      <c r="E13">
+        <v>5.262627670368206</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" s="2">
+        <v>45918.60538612268</v>
+      </c>
+      <c r="B14">
+        <v>0.998978224924668</v>
+      </c>
+      <c r="C14">
+        <v>0.9882305156116444</v>
+      </c>
+      <c r="D14">
+        <v>0.503087201070504</v>
+      </c>
+      <c r="E14">
+        <v>5.262627670368206</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" s="2">
+        <v>45918.6059800463</v>
+      </c>
+      <c r="B15">
+        <v>0.998978224924668</v>
+      </c>
+      <c r="C15">
+        <v>0.9882305156116444</v>
+      </c>
+      <c r="D15">
+        <v>0.503087201070504</v>
+      </c>
+      <c r="E15">
+        <v>5.262627670368206</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" s="2">
+        <v>45918.60602019676</v>
+      </c>
+      <c r="B16">
+        <v>0.998978224924668</v>
+      </c>
+      <c r="C16">
+        <v>0.9882305156116444</v>
+      </c>
+      <c r="D16">
+        <v>0.503087201070504</v>
+      </c>
+      <c r="E16">
+        <v>5.262627670368206</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" s="2">
+        <v>45918.60836225694</v>
+      </c>
+      <c r="B17">
+        <v>0.998978224924668</v>
+      </c>
+      <c r="C17">
+        <v>0.9882305156116444</v>
+      </c>
+      <c r="D17">
+        <v>0.503087201070504</v>
+      </c>
+      <c r="E17">
+        <v>5.262627670368206</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" s="2">
+        <v>45918.6084359375</v>
+      </c>
+      <c r="B18">
+        <v>0.998978224924668</v>
+      </c>
+      <c r="C18">
+        <v>0.9882305156116444</v>
+      </c>
+      <c r="D18">
+        <v>0.503087201070504</v>
+      </c>
+      <c r="E18">
+        <v>5.262627670368206</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19" s="2">
+        <v>45918.61073287037</v>
+      </c>
+      <c r="B19">
+        <v>0.998978224924668</v>
+      </c>
+      <c r="C19">
+        <v>0.9882305156116444</v>
+      </c>
+      <c r="D19">
+        <v>0.503087201070504</v>
+      </c>
+      <c r="E19">
+        <v>5.262627670368206</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20" s="2">
+        <v>45918.61248508102</v>
+      </c>
+      <c r="B20">
+        <v>0.998978224924668</v>
+      </c>
+      <c r="C20">
+        <v>0.9882305156116444</v>
+      </c>
+      <c r="D20">
+        <v>0.503087201070504</v>
+      </c>
+      <c r="E20">
+        <v>5.262627670368206</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21" s="2">
+        <v>45918.61253494213</v>
+      </c>
+      <c r="B21">
+        <v>0.998978224924668</v>
+      </c>
+      <c r="C21">
+        <v>0.9882305156116444</v>
+      </c>
+      <c r="D21">
+        <v>0.503087201070504</v>
+      </c>
+      <c r="E21">
+        <v>5.262627670368206</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22" s="2">
+        <v>45918.61459072916</v>
+      </c>
+      <c r="B22">
+        <v>0.998978224924668</v>
+      </c>
+      <c r="C22">
+        <v>0.9882305156116444</v>
+      </c>
+      <c r="D22">
+        <v>0.503087201070504</v>
+      </c>
+      <c r="E22">
+        <v>5.262627670368206</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23" s="2">
+        <v>45918.61562175926</v>
+      </c>
+      <c r="B23">
+        <v>0.9997224718925397</v>
+      </c>
+      <c r="C23">
+        <v>0.99798780395391</v>
+      </c>
+      <c r="D23">
+        <v>0.1366453754562611</v>
+      </c>
+      <c r="E23">
+        <v>0.8997368313633023</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24" s="2">
+        <v>45918.61597215278</v>
+      </c>
+      <c r="B24">
+        <v>0.9997224718925397</v>
+      </c>
+      <c r="C24">
+        <v>0.99798780395391</v>
+      </c>
+      <c r="D24">
+        <v>0.1366453754562611</v>
+      </c>
+      <c r="E24">
+        <v>0.8997368313633023</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="A25" s="2">
+        <v>45918.61884633102</v>
+      </c>
+      <c r="B25">
+        <v>0.99972943470588</v>
+      </c>
+      <c r="C25">
+        <v>0.998022264991768</v>
+      </c>
+      <c r="D25">
+        <v>0.133217123623192</v>
+      </c>
+      <c r="E25">
+        <v>0.8843278631028983</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="A26" s="2">
+        <v>45918.61909472222</v>
+      </c>
+      <c r="B26">
+        <v>0.99972943470588</v>
+      </c>
+      <c r="C26">
+        <v>0.998022264991768</v>
+      </c>
+      <c r="D26">
+        <v>0.133217123623192</v>
+      </c>
+      <c r="E26">
+        <v>0.8843278631028983</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
+      <c r="A27" s="2">
+        <v>45918.62302925926</v>
+      </c>
+      <c r="B27">
+        <v>0.99972943470588</v>
+      </c>
+      <c r="C27">
+        <v>0.998022264991768</v>
+      </c>
+      <c r="D27">
+        <v>0.133217123623192</v>
+      </c>
+      <c r="E27">
+        <v>0.8843278631028983</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5">
+      <c r="A28" s="2">
+        <v>45918.62312708333</v>
+      </c>
+      <c r="B28">
+        <v>0.99972943470588</v>
+      </c>
+      <c r="C28">
+        <v>0.998022264991768</v>
+      </c>
+      <c r="D28">
+        <v>0.133217123623192</v>
+      </c>
+      <c r="E28">
+        <v>0.8843278631028983</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5">
+      <c r="A29" s="2">
+        <v>45918.62319002315</v>
+      </c>
+      <c r="B29">
+        <v>0.99972943470588</v>
+      </c>
+      <c r="C29">
+        <v>0.998022264991768</v>
+      </c>
+      <c r="D29">
+        <v>0.133217123623192</v>
+      </c>
+      <c r="E29">
+        <v>0.8843278631028983</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5">
+      <c r="A30" s="2">
+        <v>45918.62340684028</v>
+      </c>
+      <c r="B30">
+        <v>0.99972943470588</v>
+      </c>
+      <c r="C30">
+        <v>0.998022264991768</v>
+      </c>
+      <c r="D30">
+        <v>0.133217123623192</v>
+      </c>
+      <c r="E30">
+        <v>0.8843278631028983</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5">
+      <c r="A31" s="2">
+        <v>45918.62381653935</v>
+      </c>
+      <c r="B31">
+        <v>0.99972943470588</v>
+      </c>
+      <c r="C31">
+        <v>0.998022264991768</v>
+      </c>
+      <c r="D31">
+        <v>0.133217123623192</v>
+      </c>
+      <c r="E31">
+        <v>0.8843278631028983</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5">
+      <c r="A32" s="2">
+        <v>45918.62709280093</v>
+      </c>
+      <c r="B32">
+        <v>0.99972943470588</v>
+      </c>
+      <c r="C32">
+        <v>0.998022264991768</v>
+      </c>
+      <c r="D32">
+        <v>0.133217123623192</v>
+      </c>
+      <c r="E32">
+        <v>0.8843278631028983</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5">
+      <c r="A33" s="2">
+        <v>45918.62713597222</v>
+      </c>
+      <c r="B33">
+        <v>0.99972943470588</v>
+      </c>
+      <c r="C33">
+        <v>0.998022264991768</v>
+      </c>
+      <c r="D33">
+        <v>0.133217123623192</v>
+      </c>
+      <c r="E33">
+        <v>0.8843278631028983</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5">
+      <c r="A34" s="2">
+        <v>45918.62785251158</v>
+      </c>
+      <c r="B34">
+        <v>0.99972943470588</v>
+      </c>
+      <c r="C34">
+        <v>0.998022264991768</v>
+      </c>
+      <c r="D34">
+        <v>0.133217123623192</v>
+      </c>
+      <c r="E34">
+        <v>0.8843278631028983</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5">
+      <c r="A35" s="2">
+        <v>45918.62789674768</v>
+      </c>
+      <c r="B35">
+        <v>0.99972943470588</v>
+      </c>
+      <c r="C35">
+        <v>0.998022264991768</v>
+      </c>
+      <c r="D35">
+        <v>0.133217123623192</v>
+      </c>
+      <c r="E35">
+        <v>0.8843278631028983</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5">
+      <c r="A36" s="2">
+        <v>45918.62826903935</v>
+      </c>
+      <c r="B36">
+        <v>0.99972943470588</v>
+      </c>
+      <c r="C36">
+        <v>0.998022264991768</v>
+      </c>
+      <c r="D36">
+        <v>0.133217123623192</v>
+      </c>
+      <c r="E36">
+        <v>0.8843278631028983</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5">
+      <c r="A37" s="2">
+        <v>45918.62831399305</v>
+      </c>
+      <c r="B37">
+        <v>0.99972943470588</v>
+      </c>
+      <c r="C37">
+        <v>0.998022264991768</v>
+      </c>
+      <c r="D37">
+        <v>0.133217123623192</v>
+      </c>
+      <c r="E37">
+        <v>0.8843278631028983</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5">
+      <c r="A38" s="2">
+        <v>45918.62857828704</v>
+      </c>
+      <c r="B38">
+        <v>0.99972943470588</v>
+      </c>
+      <c r="C38">
+        <v>0.998022264991768</v>
+      </c>
+      <c r="D38">
+        <v>0.133217123623192</v>
+      </c>
+      <c r="E38">
+        <v>0.8843278631028983</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5">
+      <c r="A39" s="2">
+        <v>45918.62868987268</v>
+      </c>
+      <c r="B39">
+        <v>0.99972943470588</v>
+      </c>
+      <c r="C39">
+        <v>0.998022264991768</v>
+      </c>
+      <c r="D39">
+        <v>0.133217123623192</v>
+      </c>
+      <c r="E39">
+        <v>0.8843278631028983</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5">
+      <c r="A40" s="2">
+        <v>45918.62871054398</v>
+      </c>
+      <c r="B40">
+        <v>0.99972943470588</v>
+      </c>
+      <c r="C40">
+        <v>0.998022264991768</v>
+      </c>
+      <c r="D40">
+        <v>0.133217123623192</v>
+      </c>
+      <c r="E40">
+        <v>0.8843278631028983</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5">
+      <c r="A41" s="2">
+        <v>45918.62887842592</v>
+      </c>
+      <c r="B41">
+        <v>0.99972943470588</v>
+      </c>
+      <c r="C41">
+        <v>0.998022264991768</v>
+      </c>
+      <c r="D41">
+        <v>0.133217123623192</v>
+      </c>
+      <c r="E41">
+        <v>0.8843278631028983</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5">
+      <c r="A42" s="2">
+        <v>45918.63098435185</v>
+      </c>
+      <c r="B42">
+        <v>0.99972943470588</v>
+      </c>
+      <c r="C42">
+        <v>0.998022264991768</v>
+      </c>
+      <c r="D42">
+        <v>0.133217123623192</v>
+      </c>
+      <c r="E42">
+        <v>0.8843278631028983</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5">
+      <c r="A43" s="2">
+        <v>45918.63104008102</v>
+      </c>
+      <c r="B43">
+        <v>0.99972943470588</v>
+      </c>
+      <c r="C43">
+        <v>0.998022264991768</v>
+      </c>
+      <c r="D43">
+        <v>0.133217123623192</v>
+      </c>
+      <c r="E43">
+        <v>0.8843278631028983</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5">
+      <c r="A44" s="2">
+        <v>45918.63207424768</v>
+      </c>
+      <c r="B44">
+        <v>0.99972943470588</v>
+      </c>
+      <c r="C44">
+        <v>0.998022264991768</v>
+      </c>
+      <c r="D44">
+        <v>0.133217123623192</v>
+      </c>
+      <c r="E44">
+        <v>0.8843278631028983</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5">
+      <c r="A45" s="2">
+        <v>45918.63216040509</v>
+      </c>
+      <c r="B45">
+        <v>0.99972943470588</v>
+      </c>
+      <c r="C45">
+        <v>0.998022264991768</v>
+      </c>
+      <c r="D45">
+        <v>0.133217123623192</v>
+      </c>
+      <c r="E45">
+        <v>0.8843278631028983</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5">
+      <c r="A46" s="2">
+        <v>45918.63694368055</v>
+      </c>
+      <c r="B46">
+        <v>0.9997279674300568</v>
+      </c>
+      <c r="C46">
+        <v>0.9980249729134893</v>
+      </c>
+      <c r="D46">
+        <v>0.1339395601994786</v>
+      </c>
+      <c r="E46">
+        <v>0.8831170382860067</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5">
+      <c r="A47" s="2">
+        <v>45918.63710767361</v>
+      </c>
+      <c r="B47">
+        <v>0.9997279674300568</v>
+      </c>
+      <c r="C47">
+        <v>0.9980249729134893</v>
+      </c>
+      <c r="D47">
+        <v>0.1339395601994786</v>
+      </c>
+      <c r="E47">
+        <v>0.8831170382860067</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5">
+      <c r="A48" s="2">
+        <v>45918.63714979167</v>
+      </c>
+      <c r="B48">
+        <v>0.9997279674300568</v>
+      </c>
+      <c r="C48">
+        <v>0.9980249729134893</v>
+      </c>
+      <c r="D48">
+        <v>0.1339395601994786</v>
+      </c>
+      <c r="E48">
+        <v>0.8831170382860067</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5">
+      <c r="A49" s="2">
+        <v>45918.63717101852</v>
+      </c>
+      <c r="B49">
+        <v>0.9997279674300568</v>
+      </c>
+      <c r="C49">
+        <v>0.9980249729134893</v>
+      </c>
+      <c r="D49">
+        <v>0.1339395601994786</v>
+      </c>
+      <c r="E49">
+        <v>0.8831170382860067</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5">
+      <c r="A50" s="2">
+        <v>45918.64224550926</v>
+      </c>
+      <c r="B50">
+        <v>0.9997279674300568</v>
+      </c>
+      <c r="C50">
+        <v>0.9980249729134893</v>
+      </c>
+      <c r="D50">
+        <v>0.1339395601994786</v>
+      </c>
+      <c r="E50">
+        <v>0.8831170382860067</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5">
+      <c r="A51" s="2">
+        <v>45918.64228483797</v>
+      </c>
+      <c r="B51">
+        <v>0.9997279674300568</v>
+      </c>
+      <c r="C51">
+        <v>0.9980249729134893</v>
+      </c>
+      <c r="D51">
+        <v>0.1339395601994786</v>
+      </c>
+      <c r="E51">
+        <v>0.8831170382860067</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5">
+      <c r="A52" s="2">
+        <v>45918.64426923611</v>
+      </c>
+      <c r="B52">
+        <v>0.9997279674300568</v>
+      </c>
+      <c r="C52">
+        <v>0.9980249729134893</v>
+      </c>
+      <c r="D52">
+        <v>0.1339395601994786</v>
+      </c>
+      <c r="E52">
+        <v>0.8831170382860067</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5">
+      <c r="A53" s="2">
+        <v>45918.64431165509</v>
+      </c>
+      <c r="B53">
+        <v>0.9997279674300568</v>
+      </c>
+      <c r="C53">
+        <v>0.9980249729134893</v>
+      </c>
+      <c r="D53">
+        <v>0.1339395601994786</v>
+      </c>
+      <c r="E53">
+        <v>0.8831170382860067</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5">
+      <c r="A54" s="2">
+        <v>45918.64537212963</v>
+      </c>
+      <c r="B54">
+        <v>0.9997279674300568</v>
+      </c>
+      <c r="C54">
+        <v>0.9980249729134893</v>
+      </c>
+      <c r="D54">
+        <v>0.1339395601994786</v>
+      </c>
+      <c r="E54">
+        <v>0.8831170382860067</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5">
+      <c r="A55" s="2">
+        <v>45918.64541651621</v>
+      </c>
+      <c r="B55">
+        <v>0.9997279674300568</v>
+      </c>
+      <c r="C55">
+        <v>0.9980249729134893</v>
+      </c>
+      <c r="D55">
+        <v>0.1339395601994786</v>
+      </c>
+      <c r="E55">
+        <v>0.8831170382860067</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5">
+      <c r="A56" s="2">
+        <v>45918.64614525463</v>
+      </c>
+      <c r="B56">
+        <v>0.9997279674300568</v>
+      </c>
+      <c r="C56">
+        <v>0.9980249729134893</v>
+      </c>
+      <c r="D56">
+        <v>0.1339395601994786</v>
+      </c>
+      <c r="E56">
+        <v>0.8831170382860067</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5">
+      <c r="A57" s="2">
+        <v>45918.64619288195</v>
+      </c>
+      <c r="B57">
+        <v>0.9997279674300568</v>
+      </c>
+      <c r="C57">
+        <v>0.9980249729134893</v>
+      </c>
+      <c r="D57">
+        <v>0.1339395601994786</v>
+      </c>
+      <c r="E57">
+        <v>0.8831170382860067</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5">
+      <c r="A58" s="2">
+        <v>45918.64635868055</v>
+      </c>
+      <c r="B58">
+        <v>0.9997279674300568</v>
+      </c>
+      <c r="C58">
+        <v>0.9980249729134893</v>
+      </c>
+      <c r="D58">
+        <v>0.1339395601994786</v>
+      </c>
+      <c r="E58">
+        <v>0.8831170382860067</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5">
+      <c r="A59" s="2">
+        <v>45918.64641685185</v>
+      </c>
+      <c r="B59">
+        <v>0.9997279674300568</v>
+      </c>
+      <c r="C59">
+        <v>0.9980249729134893</v>
+      </c>
+      <c r="D59">
+        <v>0.1339395601994786</v>
+      </c>
+      <c r="E59">
+        <v>0.8831170382860067</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5">
+      <c r="A60" s="2">
+        <v>45918.64643289352</v>
+      </c>
+      <c r="B60">
+        <v>0.9997279674300568</v>
+      </c>
+      <c r="C60">
+        <v>0.9980249729134893</v>
+      </c>
+      <c r="D60">
+        <v>0.1339395601994786</v>
+      </c>
+      <c r="E60">
+        <v>0.8831170382860067</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5">
+      <c r="A61" s="2">
+        <v>45918.65562918982</v>
+      </c>
+      <c r="B61">
+        <v>0.9997279674300568</v>
+      </c>
+      <c r="C61">
+        <v>0.9980249729134893</v>
+      </c>
+      <c r="D61">
+        <v>0.1339395601994786</v>
+      </c>
+      <c r="E61">
+        <v>0.8831170382860067</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5">
+      <c r="A62" s="2">
+        <v>45918.68511694444</v>
+      </c>
+      <c r="B62">
+        <v>0.9997279674300568</v>
+      </c>
+      <c r="C62">
+        <v>0.9980249729134893</v>
+      </c>
+      <c r="D62">
+        <v>0.1339395601994786</v>
+      </c>
+      <c r="E62">
+        <v>0.8831170382860067</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5">
+      <c r="A63" s="2">
+        <v>45918.68525549769</v>
+      </c>
+      <c r="B63">
+        <v>0.9997279674300568</v>
+      </c>
+      <c r="C63">
+        <v>0.9980249729134893</v>
+      </c>
+      <c r="D63">
+        <v>0.1339395601994786</v>
+      </c>
+      <c r="E63">
+        <v>0.8831170382860067</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5">
+      <c r="A64" s="2">
+        <v>45918.68638611111</v>
+      </c>
+      <c r="B64">
+        <v>0.9997279674300568</v>
+      </c>
+      <c r="C64">
+        <v>0.9980249729134893</v>
+      </c>
+      <c r="D64">
+        <v>0.1339395601994786</v>
+      </c>
+      <c r="E64">
+        <v>0.8831170382860067</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5">
+      <c r="A65" s="2">
+        <v>45918.68682112268</v>
+      </c>
+      <c r="B65">
+        <v>0.9997279674300568</v>
+      </c>
+      <c r="C65">
+        <v>0.9980249729134893</v>
+      </c>
+      <c r="D65">
+        <v>0.1339395601994786</v>
+      </c>
+      <c r="E65">
+        <v>0.8831170382860067</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5">
+      <c r="A66" s="2">
+        <v>45918.68694957176</v>
+      </c>
+      <c r="B66">
+        <v>0.9997279674300568</v>
+      </c>
+      <c r="C66">
+        <v>0.9980249729134893</v>
+      </c>
+      <c r="D66">
+        <v>0.1339395601994786</v>
+      </c>
+      <c r="E66">
+        <v>0.8831170382860067</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5">
+      <c r="A67" s="2">
+        <v>45918.68813023148</v>
+      </c>
+      <c r="B67">
+        <v>0.9997279674300568</v>
+      </c>
+      <c r="C67">
+        <v>0.9980249729134893</v>
+      </c>
+      <c r="D67">
+        <v>0.1339395601994786</v>
+      </c>
+      <c r="E67">
+        <v>0.8831170382860067</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5">
+      <c r="A68" s="2">
+        <v>45918.68817765046</v>
+      </c>
+      <c r="B68">
+        <v>0.9997279674300568</v>
+      </c>
+      <c r="C68">
+        <v>0.9980249729134893</v>
+      </c>
+      <c r="D68">
+        <v>0.1339395601994786</v>
+      </c>
+      <c r="E68">
+        <v>0.8831170382860067</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5">
+      <c r="A69" s="2">
+        <v>45918.68830291666</v>
+      </c>
+      <c r="B69">
+        <v>0.9997279674300568</v>
+      </c>
+      <c r="C69">
+        <v>0.9980249729134893</v>
+      </c>
+      <c r="D69">
+        <v>0.1339395601994786</v>
+      </c>
+      <c r="E69">
+        <v>0.8831170382860067</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5">
+      <c r="A70" s="2">
+        <v>45918.71943976852</v>
+      </c>
+      <c r="B70">
+        <v>0.9997279674300568</v>
+      </c>
+      <c r="C70">
+        <v>0.9980249729134893</v>
+      </c>
+      <c r="D70">
+        <v>0.1339395601994786</v>
+      </c>
+      <c r="E70">
+        <v>0.8831170382860067</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5">
+      <c r="A71" s="2">
+        <v>45918.71950760417</v>
+      </c>
+      <c r="B71">
+        <v>0.9997279674300568</v>
+      </c>
+      <c r="C71">
+        <v>0.9980249729134893</v>
+      </c>
+      <c r="D71">
+        <v>0.1339395601994786</v>
+      </c>
+      <c r="E71">
+        <v>0.8831170382860067</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5">
+      <c r="A72" s="2">
+        <v>45918.71974424768</v>
+      </c>
+      <c r="B72">
+        <v>0.9997279674300568</v>
+      </c>
+      <c r="C72">
+        <v>0.9980249729134893</v>
+      </c>
+      <c r="D72">
+        <v>0.1339395601994786</v>
+      </c>
+      <c r="E72">
+        <v>0.8831170382860067</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5">
+      <c r="A73" s="2">
+        <v>45918.71983806713</v>
+      </c>
+      <c r="B73">
+        <v>0.9997279674300568</v>
+      </c>
+      <c r="C73">
+        <v>0.9980249729134893</v>
+      </c>
+      <c r="D73">
+        <v>0.1339395601994786</v>
+      </c>
+      <c r="E73">
+        <v>0.8831170382860067</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5">
+      <c r="A74" s="2">
+        <v>45918.72188333333</v>
+      </c>
+      <c r="B74">
+        <v>0.9997279674300568</v>
+      </c>
+      <c r="C74">
+        <v>0.9980249729134893</v>
+      </c>
+      <c r="D74">
+        <v>0.1339395601994786</v>
+      </c>
+      <c r="E74">
+        <v>0.8831170382860067</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5">
+      <c r="A75" s="2">
+        <v>45918.72201630787</v>
+      </c>
+      <c r="B75">
+        <v>0.9997279674300568</v>
+      </c>
+      <c r="C75">
+        <v>0.9980249729134893</v>
+      </c>
+      <c r="D75">
+        <v>0.1339395601994786</v>
+      </c>
+      <c r="E75">
+        <v>0.8831170382860067</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5">
+      <c r="A76" s="2">
+        <v>45918.83985798611</v>
+      </c>
+      <c r="B76">
+        <v>0.9997279674300568</v>
+      </c>
+      <c r="C76">
+        <v>0.9980249729134893</v>
+      </c>
+      <c r="D76">
+        <v>0.1339395601994786</v>
+      </c>
+      <c r="E76">
+        <v>0.8831170382860067</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5">
+      <c r="A77" s="2">
+        <v>45918.84004075231</v>
+      </c>
+      <c r="B77">
+        <v>0.9997279674300568</v>
+      </c>
+      <c r="C77">
+        <v>0.9980249729134893</v>
+      </c>
+      <c r="D77">
+        <v>0.1339395601994786</v>
+      </c>
+      <c r="E77">
+        <v>0.8831170382860067</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5">
+      <c r="A78" s="2">
+        <v>45918.84296325232</v>
+      </c>
+      <c r="B78">
+        <v>0.9997279674300568</v>
+      </c>
+      <c r="C78">
+        <v>0.9980249729134893</v>
+      </c>
+      <c r="D78">
+        <v>0.1339395601994786</v>
+      </c>
+      <c r="E78">
+        <v>0.8831170382860067</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5">
+      <c r="A79" s="2">
+        <v>45918.84306885417</v>
+      </c>
+      <c r="B79">
+        <v>0.9997279674300568</v>
+      </c>
+      <c r="C79">
+        <v>0.9980249729134893</v>
+      </c>
+      <c r="D79">
+        <v>0.1339395601994786</v>
+      </c>
+      <c r="E79">
+        <v>0.8831170382860067</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5">
+      <c r="A80" s="2">
+        <v>45918.85041084491</v>
+      </c>
+      <c r="B80">
+        <v>0.9997279674300568</v>
+      </c>
+      <c r="C80">
+        <v>0.9980249729134893</v>
+      </c>
+      <c r="D80">
+        <v>0.1339395601994786</v>
+      </c>
+      <c r="E80">
+        <v>0.8831170382860067</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5">
+      <c r="A81" s="2">
+        <v>45918.85047443287</v>
+      </c>
+      <c r="B81">
+        <v>0.9997279674300568</v>
+      </c>
+      <c r="C81">
+        <v>0.9980249729134893</v>
+      </c>
+      <c r="D81">
+        <v>0.1339395601994786</v>
+      </c>
+      <c r="E81">
+        <v>0.8831170382860067</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5">
+      <c r="A82" s="2">
+        <v>45919.60424774305</v>
+      </c>
+      <c r="B82">
+        <v>0.9997279674300568</v>
+      </c>
+      <c r="C82">
+        <v>0.9980249729134893</v>
+      </c>
+      <c r="D82">
+        <v>0.1339395601994786</v>
+      </c>
+      <c r="E82">
+        <v>0.8831170382860067</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5">
+      <c r="A83" s="2">
+        <v>45919.62038115741</v>
+      </c>
+      <c r="B83">
+        <v>0.9997279674300568</v>
+      </c>
+      <c r="C83">
+        <v>0.9980249729134893</v>
+      </c>
+      <c r="D83">
+        <v>0.1339395601994786</v>
+      </c>
+      <c r="E83">
+        <v>0.8831170382860067</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5">
+      <c r="A84" s="2">
+        <v>45919.62061841435</v>
+      </c>
+      <c r="B84">
+        <v>0.9997279674300568</v>
+      </c>
+      <c r="C84">
+        <v>0.9980249729134893</v>
+      </c>
+      <c r="D84">
+        <v>0.1339395601994786</v>
+      </c>
+      <c r="E84">
+        <v>0.8831170382860067</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5">
+      <c r="A85" s="2">
+        <v>45919.62096456018</v>
+      </c>
+      <c r="B85">
+        <v>0.9997279674300568</v>
+      </c>
+      <c r="C85">
+        <v>0.9980249729134893</v>
+      </c>
+      <c r="D85">
+        <v>0.1339395601994786</v>
+      </c>
+      <c r="E85">
+        <v>0.8831170382860067</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5">
+      <c r="A86" s="2">
+        <v>45919.62169126157</v>
+      </c>
+      <c r="B86">
+        <v>0.9997279674300568</v>
+      </c>
+      <c r="C86">
+        <v>0.9980249729134893</v>
+      </c>
+      <c r="D86">
+        <v>0.1339395601994786</v>
+      </c>
+      <c r="E86">
+        <v>0.8831170382860067</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5">
+      <c r="A87" s="2">
+        <v>45919.62184478009</v>
+      </c>
+      <c r="B87">
+        <v>0.9997279674300568</v>
+      </c>
+      <c r="C87">
+        <v>0.9980249729134893</v>
+      </c>
+      <c r="D87">
+        <v>0.1339395601994786</v>
+      </c>
+      <c r="E87">
+        <v>0.8831170382860067</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5">
+      <c r="A88" s="2">
+        <v>45919.62189800926</v>
+      </c>
+      <c r="B88">
+        <v>0.9997279674300568</v>
+      </c>
+      <c r="C88">
+        <v>0.9980249729134893</v>
+      </c>
+      <c r="D88">
+        <v>0.1339395601994786</v>
+      </c>
+      <c r="E88">
+        <v>0.8831170382860067</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5">
+      <c r="A89" s="2">
+        <v>45919.62208225694</v>
+      </c>
+      <c r="B89">
+        <v>0.9997279674300568</v>
+      </c>
+      <c r="C89">
+        <v>0.9980249729134893</v>
+      </c>
+      <c r="D89">
+        <v>0.1339395601994786</v>
+      </c>
+      <c r="E89">
+        <v>0.8831170382860067</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5">
+      <c r="A90" s="2">
+        <v>45919.62216351798</v>
+      </c>
+      <c r="B90">
+        <v>0.9997279674300568</v>
+      </c>
+      <c r="C90">
+        <v>0.9980249729134893</v>
+      </c>
+      <c r="D90">
+        <v>0.1339395601994786</v>
+      </c>
+      <c r="E90">
+        <v>0.8831170382860067</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
changes new 29th sep
</commit_message>
<xml_diff>
--- a/model_accuracy_log.xlsx
+++ b/model_accuracy_log.xlsx
@@ -390,7 +390,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E90"/>
+  <dimension ref="A1:E215"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1911,7 +1911,7 @@
     </row>
     <row r="90" spans="1:5">
       <c r="A90" s="2">
-        <v>45919.62216351798</v>
+        <v>45919.62216351852</v>
       </c>
       <c r="B90">
         <v>0.9997279674300568</v>
@@ -1924,6 +1924,2131 @@
       </c>
       <c r="E90">
         <v>0.8831170382860067</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5">
+      <c r="A91" s="2">
+        <v>45924.03677908565</v>
+      </c>
+      <c r="B91">
+        <v>0.9983066050828403</v>
+      </c>
+      <c r="C91">
+        <v>0.9982363052390251</v>
+      </c>
+      <c r="D91">
+        <v>298.7911470361831</v>
+      </c>
+      <c r="E91">
+        <v>379.1085420248258</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5">
+      <c r="A92" s="2">
+        <v>45924.03687361111</v>
+      </c>
+      <c r="B92">
+        <v>0.9983066050828403</v>
+      </c>
+      <c r="C92">
+        <v>0.9982363052390251</v>
+      </c>
+      <c r="D92">
+        <v>298.7911470361831</v>
+      </c>
+      <c r="E92">
+        <v>379.1085420248258</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5">
+      <c r="A93" s="2">
+        <v>45924.03698461805</v>
+      </c>
+      <c r="B93">
+        <v>0.9983066050828403</v>
+      </c>
+      <c r="C93">
+        <v>0.9982363052390251</v>
+      </c>
+      <c r="D93">
+        <v>298.7911470361831</v>
+      </c>
+      <c r="E93">
+        <v>379.1085420248258</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5">
+      <c r="A94" s="2">
+        <v>45924.03711635416</v>
+      </c>
+      <c r="B94">
+        <v>0.9978223604878625</v>
+      </c>
+      <c r="C94">
+        <v>0.9977934688347896</v>
+      </c>
+      <c r="D94">
+        <v>381.9630248894858</v>
+      </c>
+      <c r="E94">
+        <v>471.5184307230185</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5">
+      <c r="A95" s="2">
+        <v>45924.03719655093</v>
+      </c>
+      <c r="B95">
+        <v>0.9978223604878625</v>
+      </c>
+      <c r="C95">
+        <v>0.9977934688347896</v>
+      </c>
+      <c r="D95">
+        <v>381.9630248894858</v>
+      </c>
+      <c r="E95">
+        <v>471.5184307230185</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5">
+      <c r="A96" s="2">
+        <v>45924.03725894676</v>
+      </c>
+      <c r="B96">
+        <v>0.9978223604878625</v>
+      </c>
+      <c r="C96">
+        <v>0.9977934688347896</v>
+      </c>
+      <c r="D96">
+        <v>381.9630248894858</v>
+      </c>
+      <c r="E96">
+        <v>471.5184307230185</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5">
+      <c r="A97" s="2">
+        <v>45924.03774422454</v>
+      </c>
+      <c r="B97">
+        <v>0.9978223604878625</v>
+      </c>
+      <c r="C97">
+        <v>0.9977934688347896</v>
+      </c>
+      <c r="D97">
+        <v>381.9630248894858</v>
+      </c>
+      <c r="E97">
+        <v>471.5184307230185</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5">
+      <c r="A98" s="2">
+        <v>45924.03839540509</v>
+      </c>
+      <c r="B98">
+        <v>0.9978223604878625</v>
+      </c>
+      <c r="C98">
+        <v>0.9977934688347896</v>
+      </c>
+      <c r="D98">
+        <v>381.9630248894858</v>
+      </c>
+      <c r="E98">
+        <v>471.5184307230185</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5">
+      <c r="A99" s="2">
+        <v>45924.03841097222</v>
+      </c>
+      <c r="B99">
+        <v>0.9978223604878625</v>
+      </c>
+      <c r="C99">
+        <v>0.9977934688347896</v>
+      </c>
+      <c r="D99">
+        <v>381.9630248894858</v>
+      </c>
+      <c r="E99">
+        <v>471.5184307230185</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5">
+      <c r="A100" s="2">
+        <v>45924.03843450231</v>
+      </c>
+      <c r="B100">
+        <v>0.9978223604878625</v>
+      </c>
+      <c r="C100">
+        <v>0.9977934688347896</v>
+      </c>
+      <c r="D100">
+        <v>381.9630248894858</v>
+      </c>
+      <c r="E100">
+        <v>471.5184307230185</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5">
+      <c r="A101" s="2">
+        <v>45924.03846719908</v>
+      </c>
+      <c r="B101">
+        <v>0.9978223604878625</v>
+      </c>
+      <c r="C101">
+        <v>0.9977934688347896</v>
+      </c>
+      <c r="D101">
+        <v>381.9630248894858</v>
+      </c>
+      <c r="E101">
+        <v>471.5184307230185</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5">
+      <c r="A102" s="2">
+        <v>45924.03848415509</v>
+      </c>
+      <c r="B102">
+        <v>0.9978223604878625</v>
+      </c>
+      <c r="C102">
+        <v>0.9977934688347896</v>
+      </c>
+      <c r="D102">
+        <v>381.9630248894858</v>
+      </c>
+      <c r="E102">
+        <v>471.5184307230185</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5">
+      <c r="A103" s="2">
+        <v>45924.03852805556</v>
+      </c>
+      <c r="B103">
+        <v>0.9978223604878625</v>
+      </c>
+      <c r="C103">
+        <v>0.9977934688347896</v>
+      </c>
+      <c r="D103">
+        <v>381.9630248894858</v>
+      </c>
+      <c r="E103">
+        <v>471.5184307230185</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5">
+      <c r="A104" s="2">
+        <v>45924.0385767824</v>
+      </c>
+      <c r="B104">
+        <v>0.9978223604878625</v>
+      </c>
+      <c r="C104">
+        <v>0.9977934688347896</v>
+      </c>
+      <c r="D104">
+        <v>381.9630248894858</v>
+      </c>
+      <c r="E104">
+        <v>471.5184307230185</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5">
+      <c r="A105" s="2">
+        <v>45924.03886767361</v>
+      </c>
+      <c r="B105">
+        <v>0.9978223604878625</v>
+      </c>
+      <c r="C105">
+        <v>0.9977934688347896</v>
+      </c>
+      <c r="D105">
+        <v>381.9630248894858</v>
+      </c>
+      <c r="E105">
+        <v>471.5184307230185</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5">
+      <c r="A106" s="2">
+        <v>45924.03890460648</v>
+      </c>
+      <c r="B106">
+        <v>0.9978223604878625</v>
+      </c>
+      <c r="C106">
+        <v>0.9977934688347896</v>
+      </c>
+      <c r="D106">
+        <v>381.9630248894858</v>
+      </c>
+      <c r="E106">
+        <v>471.5184307230185</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5">
+      <c r="A107" s="2">
+        <v>45924.03908413195</v>
+      </c>
+      <c r="B107">
+        <v>0.9978223604878625</v>
+      </c>
+      <c r="C107">
+        <v>0.9977934688347896</v>
+      </c>
+      <c r="D107">
+        <v>381.9630248894858</v>
+      </c>
+      <c r="E107">
+        <v>471.5184307230185</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5">
+      <c r="A108" s="2">
+        <v>45924.03912216435</v>
+      </c>
+      <c r="B108">
+        <v>0.9978223604878625</v>
+      </c>
+      <c r="C108">
+        <v>0.9977934688347896</v>
+      </c>
+      <c r="D108">
+        <v>381.9630248894858</v>
+      </c>
+      <c r="E108">
+        <v>471.5184307230185</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5">
+      <c r="A109" s="2">
+        <v>45924.04062236111</v>
+      </c>
+      <c r="B109">
+        <v>0.9978223604878625</v>
+      </c>
+      <c r="C109">
+        <v>0.9977934688347896</v>
+      </c>
+      <c r="D109">
+        <v>381.9630248894858</v>
+      </c>
+      <c r="E109">
+        <v>471.5184307230185</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5">
+      <c r="A110" s="2">
+        <v>45924.04068284722</v>
+      </c>
+      <c r="B110">
+        <v>0.9978223604878625</v>
+      </c>
+      <c r="C110">
+        <v>0.9977934688347896</v>
+      </c>
+      <c r="D110">
+        <v>381.9630248894858</v>
+      </c>
+      <c r="E110">
+        <v>471.5184307230185</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5">
+      <c r="A111" s="2">
+        <v>45924.04078219907</v>
+      </c>
+      <c r="B111">
+        <v>0.9978223604878625</v>
+      </c>
+      <c r="C111">
+        <v>0.9977934688347896</v>
+      </c>
+      <c r="D111">
+        <v>381.9630248894858</v>
+      </c>
+      <c r="E111">
+        <v>471.5184307230185</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5">
+      <c r="A112" s="2">
+        <v>45924.04082140046</v>
+      </c>
+      <c r="B112">
+        <v>0.9978223604878625</v>
+      </c>
+      <c r="C112">
+        <v>0.9977934688347896</v>
+      </c>
+      <c r="D112">
+        <v>381.9630248894858</v>
+      </c>
+      <c r="E112">
+        <v>471.5184307230185</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5">
+      <c r="A113" s="2">
+        <v>45924.04094148148</v>
+      </c>
+      <c r="B113">
+        <v>0.9978223604878625</v>
+      </c>
+      <c r="C113">
+        <v>0.9977934688347896</v>
+      </c>
+      <c r="D113">
+        <v>381.9630248894858</v>
+      </c>
+      <c r="E113">
+        <v>471.5184307230185</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5">
+      <c r="A114" s="2">
+        <v>45924.04097365741</v>
+      </c>
+      <c r="B114">
+        <v>0.9978223604878625</v>
+      </c>
+      <c r="C114">
+        <v>0.9977934688347896</v>
+      </c>
+      <c r="D114">
+        <v>381.9630248894858</v>
+      </c>
+      <c r="E114">
+        <v>471.5184307230185</v>
+      </c>
+    </row>
+    <row r="115" spans="1:5">
+      <c r="A115" s="2">
+        <v>45924.04108991898</v>
+      </c>
+      <c r="B115">
+        <v>0.9978223604878625</v>
+      </c>
+      <c r="C115">
+        <v>0.9977934688347896</v>
+      </c>
+      <c r="D115">
+        <v>381.9630248894858</v>
+      </c>
+      <c r="E115">
+        <v>471.5184307230185</v>
+      </c>
+    </row>
+    <row r="116" spans="1:5">
+      <c r="A116" s="2">
+        <v>45924.04111928241</v>
+      </c>
+      <c r="B116">
+        <v>0.9978223604878625</v>
+      </c>
+      <c r="C116">
+        <v>0.9977934688347896</v>
+      </c>
+      <c r="D116">
+        <v>381.9630248894858</v>
+      </c>
+      <c r="E116">
+        <v>471.5184307230185</v>
+      </c>
+    </row>
+    <row r="117" spans="1:5">
+      <c r="A117" s="2">
+        <v>45924.04123693287</v>
+      </c>
+      <c r="B117">
+        <v>0.9978223604878625</v>
+      </c>
+      <c r="C117">
+        <v>0.9977934688347896</v>
+      </c>
+      <c r="D117">
+        <v>381.9630248894858</v>
+      </c>
+      <c r="E117">
+        <v>471.5184307230185</v>
+      </c>
+    </row>
+    <row r="118" spans="1:5">
+      <c r="A118" s="2">
+        <v>45924.04127328704</v>
+      </c>
+      <c r="B118">
+        <v>0.9978223604878625</v>
+      </c>
+      <c r="C118">
+        <v>0.9977934688347896</v>
+      </c>
+      <c r="D118">
+        <v>381.9630248894858</v>
+      </c>
+      <c r="E118">
+        <v>471.5184307230185</v>
+      </c>
+    </row>
+    <row r="119" spans="1:5">
+      <c r="A119" s="2">
+        <v>45924.04132040509</v>
+      </c>
+      <c r="B119">
+        <v>0.9978223604878625</v>
+      </c>
+      <c r="C119">
+        <v>0.9977934688347896</v>
+      </c>
+      <c r="D119">
+        <v>381.9630248894858</v>
+      </c>
+      <c r="E119">
+        <v>471.5184307230185</v>
+      </c>
+    </row>
+    <row r="120" spans="1:5">
+      <c r="A120" s="2">
+        <v>45924.0415682176</v>
+      </c>
+      <c r="B120">
+        <v>0.9978223604878625</v>
+      </c>
+      <c r="C120">
+        <v>0.9977934688347896</v>
+      </c>
+      <c r="D120">
+        <v>381.9630248894858</v>
+      </c>
+      <c r="E120">
+        <v>471.5184307230185</v>
+      </c>
+    </row>
+    <row r="121" spans="1:5">
+      <c r="A121" s="2">
+        <v>45924.04247710648</v>
+      </c>
+      <c r="B121">
+        <v>0.9978223604878625</v>
+      </c>
+      <c r="C121">
+        <v>0.9977934688347896</v>
+      </c>
+      <c r="D121">
+        <v>381.9630248894858</v>
+      </c>
+      <c r="E121">
+        <v>471.5184307230185</v>
+      </c>
+    </row>
+    <row r="122" spans="1:5">
+      <c r="A122" s="2">
+        <v>45924.04250664352</v>
+      </c>
+      <c r="B122">
+        <v>0.9978223604878625</v>
+      </c>
+      <c r="C122">
+        <v>0.9977934688347896</v>
+      </c>
+      <c r="D122">
+        <v>381.9630248894858</v>
+      </c>
+      <c r="E122">
+        <v>471.5184307230185</v>
+      </c>
+    </row>
+    <row r="123" spans="1:5">
+      <c r="A123" s="2">
+        <v>45924.04275402777</v>
+      </c>
+      <c r="B123">
+        <v>0.9978223604878625</v>
+      </c>
+      <c r="C123">
+        <v>0.9977934688347896</v>
+      </c>
+      <c r="D123">
+        <v>381.9630248894858</v>
+      </c>
+      <c r="E123">
+        <v>471.5184307230185</v>
+      </c>
+    </row>
+    <row r="124" spans="1:5">
+      <c r="A124" s="2">
+        <v>45924.04279320602</v>
+      </c>
+      <c r="B124">
+        <v>0.9978223604878625</v>
+      </c>
+      <c r="C124">
+        <v>0.9977934688347896</v>
+      </c>
+      <c r="D124">
+        <v>381.9630248894858</v>
+      </c>
+      <c r="E124">
+        <v>471.5184307230185</v>
+      </c>
+    </row>
+    <row r="125" spans="1:5">
+      <c r="A125" s="2">
+        <v>45924.04281445602</v>
+      </c>
+      <c r="B125">
+        <v>0.9978223604878625</v>
+      </c>
+      <c r="C125">
+        <v>0.9977934688347896</v>
+      </c>
+      <c r="D125">
+        <v>381.9630248894858</v>
+      </c>
+      <c r="E125">
+        <v>471.5184307230185</v>
+      </c>
+    </row>
+    <row r="126" spans="1:5">
+      <c r="A126" s="2">
+        <v>45924.04282726852</v>
+      </c>
+      <c r="B126">
+        <v>0.9978223604878625</v>
+      </c>
+      <c r="C126">
+        <v>0.9977934688347896</v>
+      </c>
+      <c r="D126">
+        <v>381.9630248894858</v>
+      </c>
+      <c r="E126">
+        <v>471.5184307230185</v>
+      </c>
+    </row>
+    <row r="127" spans="1:5">
+      <c r="A127" s="2">
+        <v>45924.04283576389</v>
+      </c>
+      <c r="B127">
+        <v>0.9978223604878625</v>
+      </c>
+      <c r="C127">
+        <v>0.9977934688347896</v>
+      </c>
+      <c r="D127">
+        <v>381.9630248894858</v>
+      </c>
+      <c r="E127">
+        <v>471.5184307230185</v>
+      </c>
+    </row>
+    <row r="128" spans="1:5">
+      <c r="A128" s="2">
+        <v>45924.04284425926</v>
+      </c>
+      <c r="B128">
+        <v>0.9978223604878625</v>
+      </c>
+      <c r="C128">
+        <v>0.9977934688347896</v>
+      </c>
+      <c r="D128">
+        <v>381.9630248894858</v>
+      </c>
+      <c r="E128">
+        <v>471.5184307230185</v>
+      </c>
+    </row>
+    <row r="129" spans="1:5">
+      <c r="A129" s="2">
+        <v>45924.04289091435</v>
+      </c>
+      <c r="B129">
+        <v>0.9978223604878625</v>
+      </c>
+      <c r="C129">
+        <v>0.9977934688347896</v>
+      </c>
+      <c r="D129">
+        <v>381.9630248894858</v>
+      </c>
+      <c r="E129">
+        <v>471.5184307230185</v>
+      </c>
+    </row>
+    <row r="130" spans="1:5">
+      <c r="A130" s="2">
+        <v>45924.04347734954</v>
+      </c>
+      <c r="B130">
+        <v>0.9978223604878625</v>
+      </c>
+      <c r="C130">
+        <v>0.9977934688347896</v>
+      </c>
+      <c r="D130">
+        <v>381.9630248894858</v>
+      </c>
+      <c r="E130">
+        <v>471.5184307230185</v>
+      </c>
+    </row>
+    <row r="131" spans="1:5">
+      <c r="A131" s="2">
+        <v>45924.04349820602</v>
+      </c>
+      <c r="B131">
+        <v>0.9978223604878625</v>
+      </c>
+      <c r="C131">
+        <v>0.9977934688347896</v>
+      </c>
+      <c r="D131">
+        <v>381.9630248894858</v>
+      </c>
+      <c r="E131">
+        <v>471.5184307230185</v>
+      </c>
+    </row>
+    <row r="132" spans="1:5">
+      <c r="A132" s="2">
+        <v>45924.04350762731</v>
+      </c>
+      <c r="B132">
+        <v>0.9978223604878625</v>
+      </c>
+      <c r="C132">
+        <v>0.9977934688347896</v>
+      </c>
+      <c r="D132">
+        <v>381.9630248894858</v>
+      </c>
+      <c r="E132">
+        <v>471.5184307230185</v>
+      </c>
+    </row>
+    <row r="133" spans="1:5">
+      <c r="A133" s="2">
+        <v>45924.04352296297</v>
+      </c>
+      <c r="B133">
+        <v>0.9978223604878625</v>
+      </c>
+      <c r="C133">
+        <v>0.9977934688347896</v>
+      </c>
+      <c r="D133">
+        <v>381.9630248894858</v>
+      </c>
+      <c r="E133">
+        <v>471.5184307230185</v>
+      </c>
+    </row>
+    <row r="134" spans="1:5">
+      <c r="A134" s="2">
+        <v>45924.0435409838</v>
+      </c>
+      <c r="B134">
+        <v>0.9978223604878625</v>
+      </c>
+      <c r="C134">
+        <v>0.9977934688347896</v>
+      </c>
+      <c r="D134">
+        <v>381.9630248894858</v>
+      </c>
+      <c r="E134">
+        <v>471.5184307230185</v>
+      </c>
+    </row>
+    <row r="135" spans="1:5">
+      <c r="A135" s="2">
+        <v>45924.04364730324</v>
+      </c>
+      <c r="B135">
+        <v>0.9978223604878625</v>
+      </c>
+      <c r="C135">
+        <v>0.9977934688347896</v>
+      </c>
+      <c r="D135">
+        <v>381.9630248894858</v>
+      </c>
+      <c r="E135">
+        <v>471.5184307230185</v>
+      </c>
+    </row>
+    <row r="136" spans="1:5">
+      <c r="A136" s="2">
+        <v>45924.04367825232</v>
+      </c>
+      <c r="B136">
+        <v>0.9978223604878625</v>
+      </c>
+      <c r="C136">
+        <v>0.9977934688347896</v>
+      </c>
+      <c r="D136">
+        <v>381.9630248894858</v>
+      </c>
+      <c r="E136">
+        <v>471.5184307230185</v>
+      </c>
+    </row>
+    <row r="137" spans="1:5">
+      <c r="A137" s="2">
+        <v>45924.0437055787</v>
+      </c>
+      <c r="B137">
+        <v>0.9978223604878625</v>
+      </c>
+      <c r="C137">
+        <v>0.9977934688347896</v>
+      </c>
+      <c r="D137">
+        <v>381.9630248894858</v>
+      </c>
+      <c r="E137">
+        <v>471.5184307230185</v>
+      </c>
+    </row>
+    <row r="138" spans="1:5">
+      <c r="A138" s="2">
+        <v>45924.04382025463</v>
+      </c>
+      <c r="B138">
+        <v>0.9978223604878625</v>
+      </c>
+      <c r="C138">
+        <v>0.9977934688347896</v>
+      </c>
+      <c r="D138">
+        <v>381.9630248894858</v>
+      </c>
+      <c r="E138">
+        <v>471.5184307230185</v>
+      </c>
+    </row>
+    <row r="139" spans="1:5">
+      <c r="A139" s="2">
+        <v>45924.04383355324</v>
+      </c>
+      <c r="B139">
+        <v>0.9978223604878625</v>
+      </c>
+      <c r="C139">
+        <v>0.9977934688347896</v>
+      </c>
+      <c r="D139">
+        <v>381.9630248894858</v>
+      </c>
+      <c r="E139">
+        <v>471.5184307230185</v>
+      </c>
+    </row>
+    <row r="140" spans="1:5">
+      <c r="A140" s="2">
+        <v>45924.0438459375</v>
+      </c>
+      <c r="B140">
+        <v>0.9978223604878625</v>
+      </c>
+      <c r="C140">
+        <v>0.9977934688347896</v>
+      </c>
+      <c r="D140">
+        <v>381.9630248894858</v>
+      </c>
+      <c r="E140">
+        <v>471.5184307230185</v>
+      </c>
+    </row>
+    <row r="141" spans="1:5">
+      <c r="A141" s="2">
+        <v>45924.04385581019</v>
+      </c>
+      <c r="B141">
+        <v>0.9978223604878625</v>
+      </c>
+      <c r="C141">
+        <v>0.9977934688347896</v>
+      </c>
+      <c r="D141">
+        <v>381.9630248894858</v>
+      </c>
+      <c r="E141">
+        <v>471.5184307230185</v>
+      </c>
+    </row>
+    <row r="142" spans="1:5">
+      <c r="A142" s="2">
+        <v>45924.04386866898</v>
+      </c>
+      <c r="B142">
+        <v>0.9978223604878625</v>
+      </c>
+      <c r="C142">
+        <v>0.9977934688347896</v>
+      </c>
+      <c r="D142">
+        <v>381.9630248894858</v>
+      </c>
+      <c r="E142">
+        <v>471.5184307230185</v>
+      </c>
+    </row>
+    <row r="143" spans="1:5">
+      <c r="A143" s="2">
+        <v>45924.0438771875</v>
+      </c>
+      <c r="B143">
+        <v>0.9978223604878625</v>
+      </c>
+      <c r="C143">
+        <v>0.9977934688347896</v>
+      </c>
+      <c r="D143">
+        <v>381.9630248894858</v>
+      </c>
+      <c r="E143">
+        <v>471.5184307230185</v>
+      </c>
+    </row>
+    <row r="144" spans="1:5">
+      <c r="A144" s="2">
+        <v>45924.04392052083</v>
+      </c>
+      <c r="B144">
+        <v>0.9978223604878625</v>
+      </c>
+      <c r="C144">
+        <v>0.9977934688347896</v>
+      </c>
+      <c r="D144">
+        <v>381.9630248894858</v>
+      </c>
+      <c r="E144">
+        <v>471.5184307230185</v>
+      </c>
+    </row>
+    <row r="145" spans="1:5">
+      <c r="A145" s="2">
+        <v>45924.04407626158</v>
+      </c>
+      <c r="B145">
+        <v>0.9978223604878625</v>
+      </c>
+      <c r="C145">
+        <v>0.9977934688347896</v>
+      </c>
+      <c r="D145">
+        <v>381.9630248894858</v>
+      </c>
+      <c r="E145">
+        <v>471.5184307230185</v>
+      </c>
+    </row>
+    <row r="146" spans="1:5">
+      <c r="A146" s="2">
+        <v>45924.04410822917</v>
+      </c>
+      <c r="B146">
+        <v>0.9978223604878625</v>
+      </c>
+      <c r="C146">
+        <v>0.9977934688347896</v>
+      </c>
+      <c r="D146">
+        <v>381.9630248894858</v>
+      </c>
+      <c r="E146">
+        <v>471.5184307230185</v>
+      </c>
+    </row>
+    <row r="147" spans="1:5">
+      <c r="A147" s="2">
+        <v>45924.04416320602</v>
+      </c>
+      <c r="B147">
+        <v>0.9978223604878625</v>
+      </c>
+      <c r="C147">
+        <v>0.9977934688347896</v>
+      </c>
+      <c r="D147">
+        <v>381.9630248894858</v>
+      </c>
+      <c r="E147">
+        <v>471.5184307230185</v>
+      </c>
+    </row>
+    <row r="148" spans="1:5">
+      <c r="A148" s="2">
+        <v>45924.04462203704</v>
+      </c>
+      <c r="B148">
+        <v>0.9978223604878625</v>
+      </c>
+      <c r="C148">
+        <v>0.9977934688347896</v>
+      </c>
+      <c r="D148">
+        <v>381.9630248894858</v>
+      </c>
+      <c r="E148">
+        <v>471.5184307230185</v>
+      </c>
+    </row>
+    <row r="149" spans="1:5">
+      <c r="A149" s="2">
+        <v>45924.04465239583</v>
+      </c>
+      <c r="B149">
+        <v>0.9978223604878625</v>
+      </c>
+      <c r="C149">
+        <v>0.9977934688347896</v>
+      </c>
+      <c r="D149">
+        <v>381.9630248894858</v>
+      </c>
+      <c r="E149">
+        <v>471.5184307230185</v>
+      </c>
+    </row>
+    <row r="150" spans="1:5">
+      <c r="A150" s="2">
+        <v>45924.04768857639</v>
+      </c>
+      <c r="B150">
+        <v>1</v>
+      </c>
+      <c r="C150">
+        <v>0.9579482551475382</v>
+      </c>
+      <c r="D150">
+        <v>3.085879060752512E-28</v>
+      </c>
+      <c r="E150">
+        <v>33.67741784596998</v>
+      </c>
+    </row>
+    <row r="151" spans="1:5">
+      <c r="A151" s="2">
+        <v>45924.04819511574</v>
+      </c>
+      <c r="B151">
+        <v>1</v>
+      </c>
+      <c r="C151">
+        <v>0.9579482551475382</v>
+      </c>
+      <c r="D151">
+        <v>3.085879060752512E-28</v>
+      </c>
+      <c r="E151">
+        <v>33.67741784596998</v>
+      </c>
+    </row>
+    <row r="152" spans="1:5">
+      <c r="A152" s="2">
+        <v>45924.048210625</v>
+      </c>
+      <c r="B152">
+        <v>1</v>
+      </c>
+      <c r="C152">
+        <v>0.9579482551475382</v>
+      </c>
+      <c r="D152">
+        <v>3.085879060752512E-28</v>
+      </c>
+      <c r="E152">
+        <v>33.67741784596998</v>
+      </c>
+    </row>
+    <row r="153" spans="1:5">
+      <c r="A153" s="2">
+        <v>45924.04822986111</v>
+      </c>
+      <c r="B153">
+        <v>1</v>
+      </c>
+      <c r="C153">
+        <v>0.9579482551475382</v>
+      </c>
+      <c r="D153">
+        <v>3.085879060752512E-28</v>
+      </c>
+      <c r="E153">
+        <v>33.67741784596998</v>
+      </c>
+    </row>
+    <row r="154" spans="1:5">
+      <c r="A154" s="2">
+        <v>45924.04824797454</v>
+      </c>
+      <c r="B154">
+        <v>1</v>
+      </c>
+      <c r="C154">
+        <v>0.9579482551475382</v>
+      </c>
+      <c r="D154">
+        <v>3.085879060752512E-28</v>
+      </c>
+      <c r="E154">
+        <v>33.67741784596998</v>
+      </c>
+    </row>
+    <row r="155" spans="1:5">
+      <c r="A155" s="2">
+        <v>45924.04841645833</v>
+      </c>
+      <c r="B155">
+        <v>1</v>
+      </c>
+      <c r="C155">
+        <v>0.9579482551475382</v>
+      </c>
+      <c r="D155">
+        <v>3.085879060752512E-28</v>
+      </c>
+      <c r="E155">
+        <v>33.67741784596998</v>
+      </c>
+    </row>
+    <row r="156" spans="1:5">
+      <c r="A156" s="2">
+        <v>45924.04844076389</v>
+      </c>
+      <c r="B156">
+        <v>1</v>
+      </c>
+      <c r="C156">
+        <v>0.9579482551475382</v>
+      </c>
+      <c r="D156">
+        <v>3.085879060752512E-28</v>
+      </c>
+      <c r="E156">
+        <v>33.67741784596998</v>
+      </c>
+    </row>
+    <row r="157" spans="1:5">
+      <c r="A157" s="2">
+        <v>45924.04847471065</v>
+      </c>
+      <c r="B157">
+        <v>1</v>
+      </c>
+      <c r="C157">
+        <v>0.9579482551475382</v>
+      </c>
+      <c r="D157">
+        <v>3.085879060752512E-28</v>
+      </c>
+      <c r="E157">
+        <v>33.67741784596998</v>
+      </c>
+    </row>
+    <row r="158" spans="1:5">
+      <c r="A158" s="2">
+        <v>45924.04849832176</v>
+      </c>
+      <c r="B158">
+        <v>1</v>
+      </c>
+      <c r="C158">
+        <v>0.9579482551475382</v>
+      </c>
+      <c r="D158">
+        <v>3.085879060752512E-28</v>
+      </c>
+      <c r="E158">
+        <v>33.67741784596998</v>
+      </c>
+    </row>
+    <row r="159" spans="1:5">
+      <c r="A159" s="2">
+        <v>45924.04866354167</v>
+      </c>
+      <c r="B159">
+        <v>1</v>
+      </c>
+      <c r="C159">
+        <v>0.9579482551475382</v>
+      </c>
+      <c r="D159">
+        <v>3.085879060752512E-28</v>
+      </c>
+      <c r="E159">
+        <v>33.67741784596998</v>
+      </c>
+    </row>
+    <row r="160" spans="1:5">
+      <c r="A160" s="2">
+        <v>45924.04869534722</v>
+      </c>
+      <c r="B160">
+        <v>1</v>
+      </c>
+      <c r="C160">
+        <v>0.9579482551475382</v>
+      </c>
+      <c r="D160">
+        <v>3.085879060752512E-28</v>
+      </c>
+      <c r="E160">
+        <v>33.67741784596998</v>
+      </c>
+    </row>
+    <row r="161" spans="1:5">
+      <c r="A161" s="2">
+        <v>45924.04878703703</v>
+      </c>
+      <c r="B161">
+        <v>1</v>
+      </c>
+      <c r="C161">
+        <v>0.9579482551475382</v>
+      </c>
+      <c r="D161">
+        <v>3.085879060752512E-28</v>
+      </c>
+      <c r="E161">
+        <v>33.67741784596998</v>
+      </c>
+    </row>
+    <row r="162" spans="1:5">
+      <c r="A162" s="2">
+        <v>45924.04881440973</v>
+      </c>
+      <c r="B162">
+        <v>1</v>
+      </c>
+      <c r="C162">
+        <v>0.9579482551475382</v>
+      </c>
+      <c r="D162">
+        <v>3.085879060752512E-28</v>
+      </c>
+      <c r="E162">
+        <v>33.67741784596998</v>
+      </c>
+    </row>
+    <row r="163" spans="1:5">
+      <c r="A163" s="2">
+        <v>45924.04896340278</v>
+      </c>
+      <c r="B163">
+        <v>1</v>
+      </c>
+      <c r="C163">
+        <v>0.9579482551475382</v>
+      </c>
+      <c r="D163">
+        <v>3.085879060752512E-28</v>
+      </c>
+      <c r="E163">
+        <v>33.67741784596998</v>
+      </c>
+    </row>
+    <row r="164" spans="1:5">
+      <c r="A164" s="2">
+        <v>45924.04901144676</v>
+      </c>
+      <c r="B164">
+        <v>1</v>
+      </c>
+      <c r="C164">
+        <v>0.9579482551475382</v>
+      </c>
+      <c r="D164">
+        <v>3.085879060752512E-28</v>
+      </c>
+      <c r="E164">
+        <v>33.67741784596998</v>
+      </c>
+    </row>
+    <row r="165" spans="1:5">
+      <c r="A165" s="2">
+        <v>45924.04914016204</v>
+      </c>
+      <c r="B165">
+        <v>1</v>
+      </c>
+      <c r="C165">
+        <v>0.9579482551475382</v>
+      </c>
+      <c r="D165">
+        <v>3.085879060752512E-28</v>
+      </c>
+      <c r="E165">
+        <v>33.67741784596998</v>
+      </c>
+    </row>
+    <row r="166" spans="1:5">
+      <c r="A166" s="2">
+        <v>45924.04917446759</v>
+      </c>
+      <c r="B166">
+        <v>1</v>
+      </c>
+      <c r="C166">
+        <v>0.9579482551475382</v>
+      </c>
+      <c r="D166">
+        <v>3.085879060752512E-28</v>
+      </c>
+      <c r="E166">
+        <v>33.67741784596998</v>
+      </c>
+    </row>
+    <row r="167" spans="1:5">
+      <c r="A167" s="2">
+        <v>45924.04930443287</v>
+      </c>
+      <c r="B167">
+        <v>1</v>
+      </c>
+      <c r="C167">
+        <v>0.9579482551475382</v>
+      </c>
+      <c r="D167">
+        <v>3.085879060752512E-28</v>
+      </c>
+      <c r="E167">
+        <v>33.67741784596998</v>
+      </c>
+    </row>
+    <row r="168" spans="1:5">
+      <c r="A168" s="2">
+        <v>45924.04933484954</v>
+      </c>
+      <c r="B168">
+        <v>1</v>
+      </c>
+      <c r="C168">
+        <v>0.9579482551475382</v>
+      </c>
+      <c r="D168">
+        <v>3.085879060752512E-28</v>
+      </c>
+      <c r="E168">
+        <v>33.67741784596998</v>
+      </c>
+    </row>
+    <row r="169" spans="1:5">
+      <c r="A169" s="2">
+        <v>45924.05223584491</v>
+      </c>
+      <c r="B169">
+        <v>1</v>
+      </c>
+      <c r="C169">
+        <v>0.9579482551475382</v>
+      </c>
+      <c r="D169">
+        <v>3.085879060752512E-28</v>
+      </c>
+      <c r="E169">
+        <v>33.67741784596998</v>
+      </c>
+    </row>
+    <row r="170" spans="1:5">
+      <c r="A170" s="2">
+        <v>45924.05225987268</v>
+      </c>
+      <c r="B170">
+        <v>1</v>
+      </c>
+      <c r="C170">
+        <v>0.9579482551475382</v>
+      </c>
+      <c r="D170">
+        <v>3.085879060752512E-28</v>
+      </c>
+      <c r="E170">
+        <v>33.67741784596998</v>
+      </c>
+    </row>
+    <row r="171" spans="1:5">
+      <c r="A171" s="2">
+        <v>45924.05229756945</v>
+      </c>
+      <c r="B171">
+        <v>1</v>
+      </c>
+      <c r="C171">
+        <v>0.9579482551475382</v>
+      </c>
+      <c r="D171">
+        <v>3.085879060752512E-28</v>
+      </c>
+      <c r="E171">
+        <v>33.67741784596998</v>
+      </c>
+    </row>
+    <row r="172" spans="1:5">
+      <c r="A172" s="2">
+        <v>45924.05231559028</v>
+      </c>
+      <c r="B172">
+        <v>1</v>
+      </c>
+      <c r="C172">
+        <v>0.9579482551475382</v>
+      </c>
+      <c r="D172">
+        <v>3.085879060752512E-28</v>
+      </c>
+      <c r="E172">
+        <v>33.67741784596998</v>
+      </c>
+    </row>
+    <row r="173" spans="1:5">
+      <c r="A173" s="2">
+        <v>45924.05233002315</v>
+      </c>
+      <c r="B173">
+        <v>1</v>
+      </c>
+      <c r="C173">
+        <v>0.9579482551475382</v>
+      </c>
+      <c r="D173">
+        <v>3.085879060752512E-28</v>
+      </c>
+      <c r="E173">
+        <v>33.67741784596998</v>
+      </c>
+    </row>
+    <row r="174" spans="1:5">
+      <c r="A174" s="2">
+        <v>45924.05235670139</v>
+      </c>
+      <c r="B174">
+        <v>1</v>
+      </c>
+      <c r="C174">
+        <v>0.9579482551475382</v>
+      </c>
+      <c r="D174">
+        <v>3.085879060752512E-28</v>
+      </c>
+      <c r="E174">
+        <v>33.67741784596998</v>
+      </c>
+    </row>
+    <row r="175" spans="1:5">
+      <c r="A175" s="2">
+        <v>45924.44462809028</v>
+      </c>
+      <c r="B175">
+        <v>0.9999029271433202</v>
+      </c>
+      <c r="C175">
+        <v>0.9962257009537037</v>
+      </c>
+      <c r="D175">
+        <v>0.06859582474520283</v>
+      </c>
+      <c r="E175">
+        <v>3.175876299044295</v>
+      </c>
+    </row>
+    <row r="176" spans="1:5">
+      <c r="A176" s="2">
+        <v>45924.44482662037</v>
+      </c>
+      <c r="B176">
+        <v>0.9999029271433202</v>
+      </c>
+      <c r="C176">
+        <v>0.9962257009537037</v>
+      </c>
+      <c r="D176">
+        <v>0.06859582474520283</v>
+      </c>
+      <c r="E176">
+        <v>3.175876299044295</v>
+      </c>
+    </row>
+    <row r="177" spans="1:5">
+      <c r="A177" s="2">
+        <v>45924.44524709491</v>
+      </c>
+      <c r="B177">
+        <v>0.9999029271433202</v>
+      </c>
+      <c r="C177">
+        <v>0.9962257009537037</v>
+      </c>
+      <c r="D177">
+        <v>0.06859582474520283</v>
+      </c>
+      <c r="E177">
+        <v>3.175876299044295</v>
+      </c>
+    </row>
+    <row r="178" spans="1:5">
+      <c r="A178" s="2">
+        <v>45924.44532128472</v>
+      </c>
+      <c r="B178">
+        <v>1</v>
+      </c>
+      <c r="C178">
+        <v>0.9579482551475382</v>
+      </c>
+      <c r="D178">
+        <v>3.085879060752512E-28</v>
+      </c>
+      <c r="E178">
+        <v>33.67741784596998</v>
+      </c>
+    </row>
+    <row r="179" spans="1:5">
+      <c r="A179" s="2">
+        <v>45924.44544533564</v>
+      </c>
+      <c r="B179">
+        <v>1</v>
+      </c>
+      <c r="C179">
+        <v>0.9579482551475382</v>
+      </c>
+      <c r="D179">
+        <v>3.085879060752512E-28</v>
+      </c>
+      <c r="E179">
+        <v>33.67741784596998</v>
+      </c>
+    </row>
+    <row r="180" spans="1:5">
+      <c r="A180" s="2">
+        <v>45924.44557366898</v>
+      </c>
+      <c r="B180">
+        <v>1</v>
+      </c>
+      <c r="C180">
+        <v>0.9579482551475382</v>
+      </c>
+      <c r="D180">
+        <v>3.085879060752512E-28</v>
+      </c>
+      <c r="E180">
+        <v>33.67741784596998</v>
+      </c>
+    </row>
+    <row r="181" spans="1:5">
+      <c r="A181" s="2">
+        <v>45924.44579982639</v>
+      </c>
+      <c r="B181">
+        <v>1</v>
+      </c>
+      <c r="C181">
+        <v>0.9579482551475382</v>
+      </c>
+      <c r="D181">
+        <v>3.085879060752512E-28</v>
+      </c>
+      <c r="E181">
+        <v>33.67741784596998</v>
+      </c>
+    </row>
+    <row r="182" spans="1:5">
+      <c r="A182" s="2">
+        <v>45924.44584880787</v>
+      </c>
+      <c r="B182">
+        <v>1</v>
+      </c>
+      <c r="C182">
+        <v>0.9579482551475382</v>
+      </c>
+      <c r="D182">
+        <v>3.085879060752512E-28</v>
+      </c>
+      <c r="E182">
+        <v>33.67741784596998</v>
+      </c>
+    </row>
+    <row r="183" spans="1:5">
+      <c r="A183" s="2">
+        <v>45924.44591980324</v>
+      </c>
+      <c r="B183">
+        <v>1</v>
+      </c>
+      <c r="C183">
+        <v>0.9579482551475382</v>
+      </c>
+      <c r="D183">
+        <v>3.085879060752512E-28</v>
+      </c>
+      <c r="E183">
+        <v>33.67741784596998</v>
+      </c>
+    </row>
+    <row r="184" spans="1:5">
+      <c r="A184" s="2">
+        <v>45924.44597581019</v>
+      </c>
+      <c r="B184">
+        <v>1</v>
+      </c>
+      <c r="C184">
+        <v>0.9579482551475382</v>
+      </c>
+      <c r="D184">
+        <v>3.085879060752512E-28</v>
+      </c>
+      <c r="E184">
+        <v>33.67741784596998</v>
+      </c>
+    </row>
+    <row r="185" spans="1:5">
+      <c r="A185" s="2">
+        <v>45924.44603998843</v>
+      </c>
+      <c r="B185">
+        <v>1</v>
+      </c>
+      <c r="C185">
+        <v>0.9579482551475382</v>
+      </c>
+      <c r="D185">
+        <v>3.085879060752512E-28</v>
+      </c>
+      <c r="E185">
+        <v>33.67741784596998</v>
+      </c>
+    </row>
+    <row r="186" spans="1:5">
+      <c r="A186" s="2">
+        <v>45924.44858143519</v>
+      </c>
+      <c r="B186">
+        <v>1</v>
+      </c>
+      <c r="C186">
+        <v>0.9579482551475382</v>
+      </c>
+      <c r="D186">
+        <v>3.085879060752512E-28</v>
+      </c>
+      <c r="E186">
+        <v>33.67741784596998</v>
+      </c>
+    </row>
+    <row r="187" spans="1:5">
+      <c r="A187" s="2">
+        <v>45924.44893210648</v>
+      </c>
+      <c r="B187">
+        <v>1</v>
+      </c>
+      <c r="C187">
+        <v>0.9579482551475382</v>
+      </c>
+      <c r="D187">
+        <v>3.085879060752512E-28</v>
+      </c>
+      <c r="E187">
+        <v>33.67741784596998</v>
+      </c>
+    </row>
+    <row r="188" spans="1:5">
+      <c r="A188" s="2">
+        <v>45924.44903989584</v>
+      </c>
+      <c r="B188">
+        <v>1</v>
+      </c>
+      <c r="C188">
+        <v>0.9579482551475382</v>
+      </c>
+      <c r="D188">
+        <v>3.085879060752512E-28</v>
+      </c>
+      <c r="E188">
+        <v>33.67741784596998</v>
+      </c>
+    </row>
+    <row r="189" spans="1:5">
+      <c r="A189" s="2">
+        <v>45924.44909741898</v>
+      </c>
+      <c r="B189">
+        <v>1</v>
+      </c>
+      <c r="C189">
+        <v>0.9579482551475382</v>
+      </c>
+      <c r="D189">
+        <v>3.085879060752512E-28</v>
+      </c>
+      <c r="E189">
+        <v>33.67741784596998</v>
+      </c>
+    </row>
+    <row r="190" spans="1:5">
+      <c r="A190" s="2">
+        <v>45924.91582194444</v>
+      </c>
+      <c r="B190">
+        <v>0.9963831386512604</v>
+      </c>
+      <c r="C190">
+        <v>0.9844441476246576</v>
+      </c>
+      <c r="D190">
+        <v>2.598257583704089</v>
+      </c>
+      <c r="E190">
+        <v>13.41481292481427</v>
+      </c>
+    </row>
+    <row r="191" spans="1:5">
+      <c r="A191" s="2">
+        <v>45924.91591554398</v>
+      </c>
+      <c r="B191">
+        <v>0.9954794312892368</v>
+      </c>
+      <c r="C191">
+        <v>0.9825430295654467</v>
+      </c>
+      <c r="D191">
+        <v>3.306176353449579</v>
+      </c>
+      <c r="E191">
+        <v>14.9544116920584</v>
+      </c>
+    </row>
+    <row r="192" spans="1:5">
+      <c r="A192" s="2">
+        <v>45924.91615648148</v>
+      </c>
+      <c r="B192">
+        <v>0.9954794312892368</v>
+      </c>
+      <c r="C192">
+        <v>0.9825430295654467</v>
+      </c>
+      <c r="D192">
+        <v>3.306176353449579</v>
+      </c>
+      <c r="E192">
+        <v>14.9544116920584</v>
+      </c>
+    </row>
+    <row r="193" spans="1:5">
+      <c r="A193" s="2">
+        <v>45924.9161902662</v>
+      </c>
+      <c r="B193">
+        <v>0.9954794312892368</v>
+      </c>
+      <c r="C193">
+        <v>0.9825430295654467</v>
+      </c>
+      <c r="D193">
+        <v>3.306176353449579</v>
+      </c>
+      <c r="E193">
+        <v>14.9544116920584</v>
+      </c>
+    </row>
+    <row r="194" spans="1:5">
+      <c r="A194" s="2">
+        <v>45924.9168997801</v>
+      </c>
+      <c r="B194">
+        <v>0.9954794312892368</v>
+      </c>
+      <c r="C194">
+        <v>0.9825430295654467</v>
+      </c>
+      <c r="D194">
+        <v>3.306176353449579</v>
+      </c>
+      <c r="E194">
+        <v>14.9544116920584</v>
+      </c>
+    </row>
+    <row r="195" spans="1:5">
+      <c r="A195" s="2">
+        <v>45924.91694188657</v>
+      </c>
+      <c r="B195">
+        <v>0.9954794312892368</v>
+      </c>
+      <c r="C195">
+        <v>0.9825430295654467</v>
+      </c>
+      <c r="D195">
+        <v>3.306176353449579</v>
+      </c>
+      <c r="E195">
+        <v>14.9544116920584</v>
+      </c>
+    </row>
+    <row r="196" spans="1:5">
+      <c r="A196" s="2">
+        <v>45924.91702924768</v>
+      </c>
+      <c r="B196">
+        <v>0.9954794312892368</v>
+      </c>
+      <c r="C196">
+        <v>0.9825430295654467</v>
+      </c>
+      <c r="D196">
+        <v>3.306176353449579</v>
+      </c>
+      <c r="E196">
+        <v>14.9544116920584</v>
+      </c>
+    </row>
+    <row r="197" spans="1:5">
+      <c r="A197" s="2">
+        <v>45924.91706625</v>
+      </c>
+      <c r="B197">
+        <v>0.9954794312892368</v>
+      </c>
+      <c r="C197">
+        <v>0.9825430295654467</v>
+      </c>
+      <c r="D197">
+        <v>3.306176353449579</v>
+      </c>
+      <c r="E197">
+        <v>14.9544116920584</v>
+      </c>
+    </row>
+    <row r="198" spans="1:5">
+      <c r="A198" s="2">
+        <v>45924.91782813657</v>
+      </c>
+      <c r="B198">
+        <v>0.9954794312892368</v>
+      </c>
+      <c r="C198">
+        <v>0.9825430295654467</v>
+      </c>
+      <c r="D198">
+        <v>3.306176353449579</v>
+      </c>
+      <c r="E198">
+        <v>14.9544116920584</v>
+      </c>
+    </row>
+    <row r="199" spans="1:5">
+      <c r="A199" s="2">
+        <v>45924.91788508102</v>
+      </c>
+      <c r="B199">
+        <v>0.9954794312892368</v>
+      </c>
+      <c r="C199">
+        <v>0.9825430295654467</v>
+      </c>
+      <c r="D199">
+        <v>3.306176353449579</v>
+      </c>
+      <c r="E199">
+        <v>14.9544116920584</v>
+      </c>
+    </row>
+    <row r="200" spans="1:5">
+      <c r="A200" s="2">
+        <v>45924.93077496528</v>
+      </c>
+      <c r="B200">
+        <v>0.995478773870644</v>
+      </c>
+      <c r="C200">
+        <v>0.9825858336373147</v>
+      </c>
+      <c r="D200">
+        <v>3.306657165034329</v>
+      </c>
+      <c r="E200">
+        <v>14.91774383406949</v>
+      </c>
+    </row>
+    <row r="201" spans="1:5">
+      <c r="A201" s="2">
+        <v>45924.93094982639</v>
+      </c>
+      <c r="B201">
+        <v>0.995478773870644</v>
+      </c>
+      <c r="C201">
+        <v>0.9825858336373147</v>
+      </c>
+      <c r="D201">
+        <v>3.306657165034329</v>
+      </c>
+      <c r="E201">
+        <v>14.91774383406949</v>
+      </c>
+    </row>
+    <row r="202" spans="1:5">
+      <c r="A202" s="2">
+        <v>45924.9320446412</v>
+      </c>
+      <c r="B202">
+        <v>0.995478773870644</v>
+      </c>
+      <c r="C202">
+        <v>0.9825858336373147</v>
+      </c>
+      <c r="D202">
+        <v>3.306657165034329</v>
+      </c>
+      <c r="E202">
+        <v>14.91774383406949</v>
+      </c>
+    </row>
+    <row r="203" spans="1:5">
+      <c r="A203" s="2">
+        <v>45924.93209194444</v>
+      </c>
+      <c r="B203">
+        <v>0.995478773870644</v>
+      </c>
+      <c r="C203">
+        <v>0.9825858336373147</v>
+      </c>
+      <c r="D203">
+        <v>3.306657165034329</v>
+      </c>
+      <c r="E203">
+        <v>14.91774383406949</v>
+      </c>
+    </row>
+    <row r="204" spans="1:5">
+      <c r="A204" s="2">
+        <v>45924.93232824074</v>
+      </c>
+      <c r="B204">
+        <v>0.995478773870644</v>
+      </c>
+      <c r="C204">
+        <v>0.9825858336373147</v>
+      </c>
+      <c r="D204">
+        <v>3.306657165034329</v>
+      </c>
+      <c r="E204">
+        <v>14.91774383406949</v>
+      </c>
+    </row>
+    <row r="205" spans="1:5">
+      <c r="A205" s="2">
+        <v>45925.59811425926</v>
+      </c>
+      <c r="B205">
+        <v>0.9963828344305037</v>
+      </c>
+      <c r="C205">
+        <v>0.9844728365137645</v>
+      </c>
+      <c r="D205">
+        <v>2.598476127853872</v>
+      </c>
+      <c r="E205">
+        <v>13.39007264886515</v>
+      </c>
+    </row>
+    <row r="206" spans="1:5">
+      <c r="A206" s="2">
+        <v>45925.59820475694</v>
+      </c>
+      <c r="B206">
+        <v>0.9963828344305037</v>
+      </c>
+      <c r="C206">
+        <v>0.9844728365137645</v>
+      </c>
+      <c r="D206">
+        <v>2.598476127853872</v>
+      </c>
+      <c r="E206">
+        <v>13.39007264886515</v>
+      </c>
+    </row>
+    <row r="207" spans="1:5">
+      <c r="A207" s="2">
+        <v>45925.59839506944</v>
+      </c>
+      <c r="B207">
+        <v>0.9963828344305037</v>
+      </c>
+      <c r="C207">
+        <v>0.9844728365137645</v>
+      </c>
+      <c r="D207">
+        <v>2.598476127853872</v>
+      </c>
+      <c r="E207">
+        <v>13.39007264886515</v>
+      </c>
+    </row>
+    <row r="208" spans="1:5">
+      <c r="A208" s="2">
+        <v>45925.59853638889</v>
+      </c>
+      <c r="B208">
+        <v>0.9963828344305037</v>
+      </c>
+      <c r="C208">
+        <v>0.9844728365137645</v>
+      </c>
+      <c r="D208">
+        <v>2.598476127853872</v>
+      </c>
+      <c r="E208">
+        <v>13.39007264886515</v>
+      </c>
+    </row>
+    <row r="209" spans="1:5">
+      <c r="A209" s="2">
+        <v>45925.59857787037</v>
+      </c>
+      <c r="B209">
+        <v>0.9963828344305037</v>
+      </c>
+      <c r="C209">
+        <v>0.9844728365137645</v>
+      </c>
+      <c r="D209">
+        <v>2.598476127853872</v>
+      </c>
+      <c r="E209">
+        <v>13.39007264886515</v>
+      </c>
+    </row>
+    <row r="210" spans="1:5">
+      <c r="A210" s="2">
+        <v>45925.59872898148</v>
+      </c>
+      <c r="B210">
+        <v>0.9963828344305037</v>
+      </c>
+      <c r="C210">
+        <v>0.9844728365137645</v>
+      </c>
+      <c r="D210">
+        <v>2.598476127853872</v>
+      </c>
+      <c r="E210">
+        <v>13.39007264886515</v>
+      </c>
+    </row>
+    <row r="211" spans="1:5">
+      <c r="A211" s="2">
+        <v>45925.59876518518</v>
+      </c>
+      <c r="B211">
+        <v>0.9963828344305037</v>
+      </c>
+      <c r="C211">
+        <v>0.9844728365137645</v>
+      </c>
+      <c r="D211">
+        <v>2.598476127853872</v>
+      </c>
+      <c r="E211">
+        <v>13.39007264886515</v>
+      </c>
+    </row>
+    <row r="212" spans="1:5">
+      <c r="A212" s="2">
+        <v>45925.59896663194</v>
+      </c>
+      <c r="B212">
+        <v>0.9963828344305037</v>
+      </c>
+      <c r="C212">
+        <v>0.9844728365137645</v>
+      </c>
+      <c r="D212">
+        <v>2.598476127853872</v>
+      </c>
+      <c r="E212">
+        <v>13.39007264886515</v>
+      </c>
+    </row>
+    <row r="213" spans="1:5">
+      <c r="A213" s="2">
+        <v>45925.59899831018</v>
+      </c>
+      <c r="B213">
+        <v>0.9963828344305037</v>
+      </c>
+      <c r="C213">
+        <v>0.9844728365137645</v>
+      </c>
+      <c r="D213">
+        <v>2.598476127853872</v>
+      </c>
+      <c r="E213">
+        <v>13.39007264886515</v>
+      </c>
+    </row>
+    <row r="214" spans="1:5">
+      <c r="A214" s="2">
+        <v>45925.59910077546</v>
+      </c>
+      <c r="B214">
+        <v>0.9963828344305037</v>
+      </c>
+      <c r="C214">
+        <v>0.9844728365137645</v>
+      </c>
+      <c r="D214">
+        <v>2.598476127853872</v>
+      </c>
+      <c r="E214">
+        <v>13.39007264886515</v>
+      </c>
+    </row>
+    <row r="215" spans="1:5">
+      <c r="A215" s="2">
+        <v>45925.59913070164</v>
+      </c>
+      <c r="B215">
+        <v>0.9963828344305037</v>
+      </c>
+      <c r="C215">
+        <v>0.9844728365137645</v>
+      </c>
+      <c r="D215">
+        <v>2.598476127853872</v>
+      </c>
+      <c r="E215">
+        <v>13.39007264886515</v>
       </c>
     </row>
   </sheetData>

</xml_diff>